<commit_message>
replace test datasets with outbreaks data
</commit_message>
<xml_diff>
--- a/inst/extdata/test.xlsx
+++ b/inst/extdata/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karimmane/Documents/Karim/LSHTM/TRACE_dev/Packages/On_my_github/readepi/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karimmane/Documents/Karim/LSHTM/TRACE_dev/Packages/On_trace_github/readepi/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9448314-0FD7-0D41-8D0D-A57E3A04D7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D170BCE-997F-F644-BCAC-98DE00A3864A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="7700" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{F38E8C35-1EC1-2E41-B395-5F2639DA45EF}"/>
+    <workbookView xWindow="6920" yWindow="4380" windowWidth="27640" windowHeight="16940" xr2:uid="{F38E8C35-1EC1-2E41-B395-5F2639DA45EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,42 +37,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
-  <si>
-    <t>site</t>
-  </si>
-  <si>
-    <t>var1</t>
-  </si>
-  <si>
-    <t>mm1</t>
-  </si>
-  <si>
-    <t>mm2</t>
-  </si>
-  <si>
-    <t>mm3</t>
-  </si>
-  <si>
-    <t>mm4</t>
-  </si>
-  <si>
-    <t>mm5</t>
-  </si>
-  <si>
-    <t>mm6</t>
-  </si>
-  <si>
-    <t>mm7</t>
-  </si>
-  <si>
-    <t>mm8</t>
-  </si>
-  <si>
-    <t>mm9</t>
-  </si>
-  <si>
-    <t>mm10</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+  <si>
+    <t>case_id</t>
+  </si>
+  <si>
+    <t>date_of_onset</t>
+  </si>
+  <si>
+    <t>date_of_hospitalisation</t>
+  </si>
+  <si>
+    <t>d1fafd</t>
+  </si>
+  <si>
+    <t>53371b</t>
+  </si>
+  <si>
+    <t>f5c3d8</t>
+  </si>
+  <si>
+    <t>6c286a</t>
+  </si>
+  <si>
+    <t>0f58c4</t>
+  </si>
+  <si>
+    <t>49731d</t>
+  </si>
+  <si>
+    <t>f9149b</t>
+  </si>
+  <si>
+    <t>881bd4</t>
+  </si>
+  <si>
+    <t>e66fa4</t>
+  </si>
+  <si>
+    <t>20b688</t>
+  </si>
+  <si>
+    <t>date_of_outcome</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>date_of_infection</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Recover</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>cases</t>
+  </si>
+  <si>
+    <t>deaths</t>
   </si>
 </sst>
 </file>
@@ -108,8 +147,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,7 +168,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -416,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -424,15 +464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482398A6-5B11-2F4B-9409-BBD2BCC31BC8}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,117 +480,249 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>45.38</v>
-      </c>
-      <c r="C2">
-        <v>52.44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>41736</v>
+      </c>
+      <c r="C2" s="1">
+        <v>41746</v>
+      </c>
+      <c r="D2" s="1">
+        <v>41748</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>35.14</v>
-      </c>
-      <c r="C3">
-        <v>42.85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>41744</v>
+      </c>
+      <c r="C3" s="1">
+        <v>41749</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1">
+        <v>41738</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4.13</v>
-      </c>
-      <c r="C4">
-        <v>13.36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>41750</v>
+      </c>
+      <c r="C4" s="1">
+        <v>41754</v>
+      </c>
+      <c r="D4" s="1">
+        <v>41759</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1">
+        <v>41747</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>413.8</v>
-      </c>
-      <c r="C5">
-        <v>336.35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41756</v>
+      </c>
+      <c r="C5" s="1">
+        <v>41756</v>
+      </c>
+      <c r="D5" s="1">
+        <v>41766</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>330.6</v>
-      </c>
-      <c r="C6">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41755</v>
+      </c>
+      <c r="C6" s="1">
+        <v>41758</v>
+      </c>
+      <c r="D6" s="1">
+        <v>41776</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1">
+        <v>41751</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>119</v>
-      </c>
-      <c r="C7">
-        <v>164.12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41754</v>
+      </c>
+      <c r="C7" s="1">
+        <v>41761</v>
+      </c>
+      <c r="D7" s="1">
+        <v>41766</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1">
+        <v>41717</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>81.91</v>
-      </c>
-      <c r="C8">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41762</v>
+      </c>
+      <c r="C8" s="1">
+        <v>41763</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>55.04</v>
-      </c>
-      <c r="C9">
-        <v>72.88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41760</v>
+      </c>
+      <c r="C9" s="1">
+        <v>41764</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1">
+        <v>41755</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>2726</v>
-      </c>
-      <c r="C10">
-        <v>30.87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41750</v>
+      </c>
+      <c r="C10" s="1">
+        <v>41765</v>
+      </c>
+      <c r="D10" s="1">
+        <v>41771</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>90.19</v>
-      </c>
-      <c r="C11">
-        <v>137.18</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>41764</v>
+      </c>
+      <c r="C11" s="1">
+        <v>41765</v>
+      </c>
+      <c r="D11" s="1">
+        <v>41773</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -560,78 +732,133 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E1EB85A-FAA5-1F4A-A2ED-023478F45578}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>27997</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>27998</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>27999</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>28000</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>28001</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>28002</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>28003</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>28004</v>
+      </c>
+      <c r="B9">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>45.38</v>
-      </c>
-      <c r="C2">
-        <v>52.44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>35.14</v>
-      </c>
-      <c r="C3">
-        <v>42.85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4.13</v>
-      </c>
-      <c r="C4">
-        <v>13.36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>413.8</v>
-      </c>
-      <c r="C5">
-        <v>336.35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>330.6</v>
-      </c>
-      <c r="C6">
-        <v>0.68</v>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>28005</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>28006</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>